<commit_message>
fixed typos, checked FMEA
</commit_message>
<xml_diff>
--- a/DesignReports/SubsystemEngineering/Airframe/FMEA/figs/FMEA Template.xlsx
+++ b/DesignReports/SubsystemEngineering/Airframe/FMEA/figs/FMEA Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kameroneves/Documents/School/School/AUVSI/auvsi_documentation_2019/DesignReports/SubsystemEngineering/Airframe/FMEA/figs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tyspo\Box\Winter2019\Capstone\auvsi_documentation_2019\DesignReports\SubsystemEngineering\Airframe\FMEA\figs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{994D5A0E-E78A-404C-A8BB-4A076454853C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F43E45B8-3F98-4FC1-985A-F85C9C4381F9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{C2D87678-4539-DF41-9663-93A6919552CE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{C2D87678-4539-DF41-9663-93A6919552CE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,6 +26,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="154">
   <si>
     <t>Component</t>
   </si>
@@ -239,24 +240,15 @@
     <t>Internal Code</t>
   </si>
   <si>
-    <t>Interfearance</t>
-  </si>
-  <si>
     <t>Settings Incorrect</t>
   </si>
   <si>
-    <t>Battery Dead</t>
-  </si>
-  <si>
     <t>Mission Failure Aircraft Loiters</t>
   </si>
   <si>
     <t>Hardware failure</t>
   </si>
   <si>
-    <t>Antanna Incorrectly Pointed</t>
-  </si>
-  <si>
     <t>Poorly Connected Electrical Joint</t>
   </si>
   <si>
@@ -365,12 +357,6 @@
     <t>Components Move</t>
   </si>
   <si>
-    <t>Flight Charictoristics Change</t>
-  </si>
-  <si>
-    <t>Parts Breaks Off</t>
-  </si>
-  <si>
     <t>Icing</t>
   </si>
   <si>
@@ -380,9 +366,6 @@
     <t>Unidentified Flying Object (UFO) Impact</t>
   </si>
   <si>
-    <t>Part poorly Attached</t>
-  </si>
-  <si>
     <t>Poor Manufacturing</t>
   </si>
   <si>
@@ -431,9 +414,6 @@
     <t>Poorly Assembled</t>
   </si>
   <si>
-    <t>Aerobatic Flight that Saturates Controller</t>
-  </si>
-  <si>
     <t>Overuse</t>
   </si>
   <si>
@@ -464,9 +444,6 @@
     <t>Train saftey pilot</t>
   </si>
   <si>
-    <t>Assigne someone to point antenna</t>
-  </si>
-  <si>
     <t>Extensive testing prior to use**</t>
   </si>
   <si>
@@ -494,7 +471,31 @@
     <t>Extensive practice</t>
   </si>
   <si>
-    <t>Perform BPS bange test</t>
+    <t>Interference</t>
+  </si>
+  <si>
+    <t>Transmittor Battery Dead</t>
+  </si>
+  <si>
+    <t>Assign someone to point antenna</t>
+  </si>
+  <si>
+    <t>Antenna Incorrectly Pointed</t>
+  </si>
+  <si>
+    <t>Aerobatic Flight Saturates Controller</t>
+  </si>
+  <si>
+    <t>Flight Characteristics Change</t>
+  </si>
+  <si>
+    <t>Parts Break Off</t>
+  </si>
+  <si>
+    <t>Part poorly attached</t>
+  </si>
+  <si>
+    <t>Perform BPS range test</t>
   </si>
 </sst>
 </file>
@@ -724,7 +725,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -736,6 +737,78 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -744,78 +817,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1188,60 +1189,60 @@
   </sheetPr>
   <dimension ref="B2:O77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="Q70" sqref="Q70"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="M71" sqref="M71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="40.6640625" customWidth="1"/>
-    <col min="4" max="4" width="34.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="10" width="5.1640625" customWidth="1"/>
-    <col min="11" max="11" width="29.83203125" customWidth="1"/>
-    <col min="12" max="15" width="4.33203125" customWidth="1"/>
+    <col min="3" max="3" width="40.625" customWidth="1"/>
+    <col min="4" max="4" width="34.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="5.125" customWidth="1"/>
+    <col min="11" max="11" width="29.875" customWidth="1"/>
+    <col min="12" max="15" width="4.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" s="1" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="23" t="s">
+    <row r="2" spans="2:15" s="1" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="E2" s="23" t="s">
+      <c r="C2" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="47" t="s">
+        <v>128</v>
+      </c>
+      <c r="E2" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="23" t="s">
+      <c r="F2" s="47" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="L2" s="23" t="s">
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
-      <c r="O2" s="23"/>
-    </row>
-    <row r="3" spans="2:15" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="23"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
+      <c r="M2" s="47"/>
+      <c r="N2" s="47"/>
+      <c r="O2" s="47"/>
+    </row>
+    <row r="3" spans="2:15" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="47"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
       <c r="G3" s="4" t="s">
         <v>5</v>
       </c>
@@ -1254,7 +1255,7 @@
       <c r="J3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="23"/>
+      <c r="K3" s="47"/>
       <c r="L3" s="4" t="s">
         <v>5</v>
       </c>
@@ -1268,21 +1269,21 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="2:15" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="26" t="s">
+    <row r="4" spans="2:15" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="37" t="s">
         <v>27</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="E4" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>71</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>74</v>
       </c>
       <c r="G4" s="3">
         <v>8</v>
@@ -1312,9 +1313,9 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="2:15" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="B5" s="27"/>
-      <c r="C5" s="30"/>
+    <row r="5" spans="2:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="35"/>
+      <c r="C5" s="38"/>
       <c r="D5" s="6" t="s">
         <v>64</v>
       </c>
@@ -1338,7 +1339,7 @@
         <v>90</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="L5" s="3">
         <v>9</v>
@@ -1354,17 +1355,17 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B6" s="28"/>
-      <c r="C6" s="31"/>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B6" s="36"/>
+      <c r="C6" s="39"/>
       <c r="D6" s="7" t="s">
         <v>65</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>68</v>
+        <v>145</v>
       </c>
       <c r="G6" s="2">
         <v>8</v>
@@ -1380,7 +1381,7 @@
         <v>288</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="L6" s="2">
         <v>8</v>
@@ -1396,21 +1397,21 @@
         <v>96</v>
       </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B7" s="32" t="s">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B7" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="35" t="s">
+      <c r="C7" s="29" t="s">
         <v>28</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E7" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="F7" s="9" t="s">
         <v>71</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>74</v>
       </c>
       <c r="G7" s="5">
         <v>8</v>
@@ -1426,7 +1427,7 @@
         <v>112</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="L7" s="5">
         <v>8</v>
@@ -1442,9 +1443,9 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B8" s="33"/>
-      <c r="C8" s="36"/>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B8" s="27"/>
+      <c r="C8" s="30"/>
       <c r="D8" s="9" t="s">
         <v>64</v>
       </c>
@@ -1452,7 +1453,7 @@
         <v>66</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G8" s="5">
         <v>9</v>
@@ -1468,7 +1469,7 @@
         <v>108</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="L8" s="5">
         <v>9</v>
@@ -1477,24 +1478,24 @@
         <v>1</v>
       </c>
       <c r="N8" s="5">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="O8" s="14">
         <f t="shared" si="1"/>
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B9" s="33"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="41" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B9" s="27"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="E9" s="41" t="s">
-        <v>71</v>
+      <c r="E9" s="32" t="s">
+        <v>69</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G9" s="5">
         <v>8</v>
@@ -1510,7 +1511,7 @@
         <v>384</v>
       </c>
       <c r="K9" s="9" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="L9" s="5">
         <v>8</v>
@@ -1526,13 +1527,13 @@
         <v>96</v>
       </c>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B10" s="33"/>
-      <c r="C10" s="36"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B10" s="27"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="46"/>
       <c r="F10" s="9" t="s">
-        <v>68</v>
+        <v>145</v>
       </c>
       <c r="G10" s="5">
         <v>8</v>
@@ -1548,7 +1549,7 @@
         <v>288</v>
       </c>
       <c r="K10" s="9" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="L10" s="5">
         <v>8</v>
@@ -1564,13 +1565,13 @@
         <v>96</v>
       </c>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B11" s="34"/>
-      <c r="C11" s="37"/>
-      <c r="D11" s="43"/>
-      <c r="E11" s="43"/>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B11" s="28"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
       <c r="F11" s="9" t="s">
-        <v>70</v>
+        <v>146</v>
       </c>
       <c r="G11" s="5">
         <v>8</v>
@@ -1586,7 +1587,7 @@
         <v>144</v>
       </c>
       <c r="K11" s="9" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="L11" s="5">
         <v>8</v>
@@ -1602,21 +1603,21 @@
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B12" s="26" t="s">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B12" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="29" t="s">
+      <c r="C12" s="37" t="s">
         <v>35</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G12" s="19">
         <v>6</v>
@@ -1646,17 +1647,17 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B13" s="28"/>
-      <c r="C13" s="31"/>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B13" s="36"/>
+      <c r="C13" s="39"/>
       <c r="D13" s="12" t="s">
         <v>65</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>73</v>
+        <v>148</v>
       </c>
       <c r="G13" s="2">
         <v>6</v>
@@ -1672,7 +1673,7 @@
         <v>126</v>
       </c>
       <c r="K13" s="7" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="L13" s="2">
         <v>6</v>
@@ -1688,21 +1689,21 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B14" s="32" t="s">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B14" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="35" t="s">
+      <c r="C14" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="41" t="s">
-        <v>72</v>
+      <c r="D14" s="32" t="s">
+        <v>70</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G14" s="5">
         <v>6</v>
@@ -1732,15 +1733,15 @@
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B15" s="34"/>
-      <c r="C15" s="37"/>
-      <c r="D15" s="43"/>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B15" s="28"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="33"/>
       <c r="E15" s="9" t="s">
         <v>66</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G15" s="5">
         <v>9</v>
@@ -1756,7 +1757,7 @@
         <v>63</v>
       </c>
       <c r="K15" s="9" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="L15" s="5">
         <v>9</v>
@@ -1772,15 +1773,15 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B16" s="26" t="s">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B16" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="29" t="s">
+      <c r="C16" s="37" t="s">
         <v>30</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>66</v>
@@ -1802,7 +1803,7 @@
         <v>162</v>
       </c>
       <c r="K16" s="7" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="L16" s="2">
         <v>9</v>
@@ -1818,17 +1819,17 @@
         <v>81</v>
       </c>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B17" s="28"/>
-      <c r="C17" s="31"/>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B17" s="36"/>
+      <c r="C17" s="39"/>
       <c r="D17" s="7" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>66</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G17" s="2">
         <v>9</v>
@@ -1844,7 +1845,7 @@
         <v>189</v>
       </c>
       <c r="K17" s="7" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="L17" s="2">
         <v>9</v>
@@ -1860,18 +1861,18 @@
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B18" s="32" t="s">
+    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B18" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="35" t="s">
+      <c r="C18" s="29" t="s">
         <v>31</v>
       </c>
       <c r="D18" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="E18" s="9" t="s">
         <v>75</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>78</v>
       </c>
       <c r="F18" s="9" t="s">
         <v>67</v>
@@ -1904,17 +1905,17 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B19" s="33"/>
-      <c r="C19" s="36"/>
-      <c r="D19" s="41" t="s">
-        <v>77</v>
-      </c>
-      <c r="E19" s="41" t="s">
-        <v>78</v>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B19" s="27"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="E19" s="32" t="s">
+        <v>75</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="G19" s="5">
         <v>4</v>
@@ -1944,13 +1945,13 @@
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B20" s="33"/>
-      <c r="C20" s="36"/>
-      <c r="D20" s="42"/>
-      <c r="E20" s="42"/>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B20" s="27"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="46"/>
+      <c r="E20" s="46"/>
       <c r="F20" s="9" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G20" s="5">
         <v>4</v>
@@ -1980,13 +1981,13 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B21" s="33"/>
-      <c r="C21" s="36"/>
-      <c r="D21" s="43"/>
-      <c r="E21" s="43"/>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B21" s="27"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="33"/>
       <c r="F21" s="9" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G21" s="5">
         <v>4</v>
@@ -2016,17 +2017,17 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B22" s="34"/>
-      <c r="C22" s="37"/>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B22" s="28"/>
+      <c r="C22" s="31"/>
       <c r="D22" s="9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G22" s="5">
         <v>4</v>
@@ -2056,15 +2057,15 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B23" s="26" t="s">
+    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B23" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="29" t="s">
+      <c r="C23" s="37" t="s">
         <v>33</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>66</v>
@@ -2086,7 +2087,7 @@
         <v>90</v>
       </c>
       <c r="K23" s="7" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="L23" s="2">
         <v>9</v>
@@ -2102,17 +2103,17 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B24" s="27"/>
-      <c r="C24" s="30"/>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B24" s="35"/>
+      <c r="C24" s="38"/>
       <c r="D24" s="7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E24" s="7" t="s">
         <v>66</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>68</v>
+        <v>145</v>
       </c>
       <c r="G24" s="2">
         <v>9</v>
@@ -2128,7 +2129,7 @@
         <v>216</v>
       </c>
       <c r="K24" s="7" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="L24" s="2">
         <v>9</v>
@@ -2144,17 +2145,17 @@
         <v>81</v>
       </c>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B25" s="28"/>
-      <c r="C25" s="31"/>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B25" s="36"/>
+      <c r="C25" s="39"/>
       <c r="D25" s="7" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E25" s="7" t="s">
         <v>66</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G25" s="2">
         <v>9</v>
@@ -2170,7 +2171,7 @@
         <v>63</v>
       </c>
       <c r="K25" s="7" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="L25" s="2">
         <v>9</v>
@@ -2186,15 +2187,15 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B26" s="32" t="s">
+    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B26" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="35" t="s">
+      <c r="C26" s="29" t="s">
         <v>36</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E26" s="9" t="s">
         <v>66</v>
@@ -2216,7 +2217,7 @@
         <v>270</v>
       </c>
       <c r="K26" s="9" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="L26" s="5">
         <v>9</v>
@@ -2232,17 +2233,17 @@
         <v>81</v>
       </c>
     </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B27" s="33"/>
-      <c r="C27" s="36"/>
+    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B27" s="27"/>
+      <c r="C27" s="30"/>
       <c r="D27" s="9" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E27" s="9" t="s">
         <v>66</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>68</v>
+        <v>145</v>
       </c>
       <c r="G27" s="5">
         <v>9</v>
@@ -2258,7 +2259,7 @@
         <v>180</v>
       </c>
       <c r="K27" s="9" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="L27" s="5">
         <v>9</v>
@@ -2274,17 +2275,17 @@
         <v>144</v>
       </c>
     </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B28" s="34"/>
-      <c r="C28" s="37"/>
+    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B28" s="28"/>
+      <c r="C28" s="31"/>
       <c r="D28" s="9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E28" s="13" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G28" s="5">
         <v>6</v>
@@ -2314,21 +2315,21 @@
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B29" s="26" t="s">
+    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B29" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="C29" s="29" t="s">
+      <c r="C29" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="D29" s="38" t="s">
-        <v>82</v>
-      </c>
-      <c r="E29" s="38" t="s">
+      <c r="D29" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="E29" s="23" t="s">
         <v>66</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G29" s="2">
         <v>9</v>
@@ -2344,7 +2345,7 @@
         <v>135</v>
       </c>
       <c r="K29" s="7" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="L29" s="2">
         <v>9</v>
@@ -2360,16 +2361,16 @@
         <v>90</v>
       </c>
     </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B30" s="27"/>
-      <c r="C30" s="30"/>
-      <c r="D30" s="39"/>
-      <c r="E30" s="39"/>
+    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B30" s="35"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="25"/>
+      <c r="E30" s="25"/>
       <c r="F30" s="7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G30" s="2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H30" s="2">
         <v>2</v>
@@ -2379,13 +2380,13 @@
       </c>
       <c r="J30" s="3">
         <f t="shared" si="0"/>
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="K30" s="7" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="L30" s="2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="M30" s="2">
         <v>1</v>
@@ -2395,16 +2396,16 @@
       </c>
       <c r="O30" s="3">
         <f t="shared" si="2"/>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B31" s="28"/>
-      <c r="C31" s="31"/>
-      <c r="D31" s="40"/>
-      <c r="E31" s="40"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B31" s="36"/>
+      <c r="C31" s="39"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="24"/>
       <c r="F31" s="7" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="G31" s="2">
         <v>9</v>
@@ -2420,7 +2421,7 @@
         <v>9</v>
       </c>
       <c r="K31" s="7" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="L31" s="2">
         <v>9</v>
@@ -2436,7 +2437,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="2:15" ht="34" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>22</v>
       </c>
@@ -2444,13 +2445,13 @@
         <v>60</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E32" s="9" t="s">
         <v>66</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G32" s="5">
         <v>9</v>
@@ -2466,7 +2467,7 @@
         <v>63</v>
       </c>
       <c r="K32" s="9" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="L32" s="5">
         <v>9</v>
@@ -2482,21 +2483,21 @@
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B33" s="26" t="s">
+    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B33" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="C33" s="29" t="s">
-        <v>87</v>
+      <c r="C33" s="37" t="s">
+        <v>84</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E33" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="F33" s="7" t="s">
         <v>94</v>
-      </c>
-      <c r="F33" s="7" t="s">
-        <v>97</v>
       </c>
       <c r="G33" s="2">
         <v>10</v>
@@ -2512,7 +2513,7 @@
         <v>150</v>
       </c>
       <c r="K33" s="7" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="L33" s="2">
         <v>10</v>
@@ -2528,17 +2529,17 @@
         <v>100</v>
       </c>
     </row>
-    <row r="34" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B34" s="27"/>
-      <c r="C34" s="30"/>
+    <row r="34" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B34" s="35"/>
+      <c r="C34" s="38"/>
       <c r="D34" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="E34" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="E34" s="7" t="s">
+      <c r="F34" s="7" t="s">
         <v>93</v>
-      </c>
-      <c r="F34" s="7" t="s">
-        <v>96</v>
       </c>
       <c r="G34" s="2">
         <v>7</v>
@@ -2554,7 +2555,7 @@
         <v>168</v>
       </c>
       <c r="K34" s="7" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="L34" s="2">
         <v>7</v>
@@ -2570,17 +2571,17 @@
         <v>70</v>
       </c>
     </row>
-    <row r="35" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B35" s="27"/>
-      <c r="C35" s="30"/>
+    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B35" s="35"/>
+      <c r="C35" s="38"/>
       <c r="D35" s="7" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E35" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="F35" s="7" t="s">
         <v>92</v>
-      </c>
-      <c r="F35" s="7" t="s">
-        <v>95</v>
       </c>
       <c r="G35" s="2">
         <v>6</v>
@@ -2595,32 +2596,34 @@
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="K35" s="7"/>
+      <c r="K35" s="7" t="s">
+        <v>131</v>
+      </c>
       <c r="L35" s="2">
         <v>6</v>
       </c>
       <c r="M35" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N35" s="2">
         <v>2</v>
       </c>
       <c r="O35" s="3">
         <f t="shared" si="2"/>
-        <v>36</v>
-      </c>
-    </row>
-    <row r="36" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B36" s="28"/>
-      <c r="C36" s="31"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B36" s="36"/>
+      <c r="C36" s="39"/>
       <c r="D36" s="7" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G36" s="2">
         <v>7</v>
@@ -2650,21 +2653,21 @@
         <v>49</v>
       </c>
     </row>
-    <row r="37" spans="2:15" ht="17" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C37" s="21" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F37" s="9" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="G37" s="5">
         <v>7</v>
@@ -2694,21 +2697,21 @@
         <v>105</v>
       </c>
     </row>
-    <row r="38" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B38" s="26" t="s">
+    <row r="38" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B38" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="C38" s="29" t="s">
+      <c r="C38" s="37" t="s">
         <v>39</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E38" s="7" t="s">
         <v>66</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="G38" s="2">
         <v>9</v>
@@ -2724,7 +2727,7 @@
         <v>504</v>
       </c>
       <c r="K38" s="7" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="L38" s="2">
         <v>9</v>
@@ -2740,17 +2743,17 @@
         <v>81</v>
       </c>
     </row>
-    <row r="39" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B39" s="27"/>
-      <c r="C39" s="30"/>
-      <c r="D39" s="38" t="s">
-        <v>100</v>
+    <row r="39" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B39" s="35"/>
+      <c r="C39" s="38"/>
+      <c r="D39" s="23" t="s">
+        <v>97</v>
       </c>
       <c r="E39" s="7" t="s">
         <v>66</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G39" s="2">
         <v>9</v>
@@ -2766,7 +2769,7 @@
         <v>216</v>
       </c>
       <c r="K39" s="7" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="L39" s="2">
         <v>9</v>
@@ -2782,15 +2785,15 @@
         <v>72</v>
       </c>
     </row>
-    <row r="40" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B40" s="28"/>
-      <c r="C40" s="31"/>
-      <c r="D40" s="40"/>
+    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B40" s="36"/>
+      <c r="C40" s="39"/>
+      <c r="D40" s="24"/>
       <c r="E40" s="7" t="s">
         <v>66</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G40" s="2">
         <v>9</v>
@@ -2806,7 +2809,7 @@
         <v>360</v>
       </c>
       <c r="K40" s="7" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="L40" s="2">
         <v>9</v>
@@ -2822,21 +2825,21 @@
         <v>72</v>
       </c>
     </row>
-    <row r="41" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B41" s="32" t="s">
+    <row r="41" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B41" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="C41" s="35" t="s">
+      <c r="C41" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="D41" s="41" t="s">
-        <v>107</v>
-      </c>
-      <c r="E41" s="41" t="s">
+      <c r="D41" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="E41" s="32" t="s">
         <v>66</v>
       </c>
       <c r="F41" s="9" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="G41" s="5">
         <v>9</v>
@@ -2845,14 +2848,14 @@
         <v>2</v>
       </c>
       <c r="I41" s="5">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J41" s="14">
         <f t="shared" si="0"/>
-        <v>144</v>
+        <v>126</v>
       </c>
       <c r="K41" s="9" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="L41" s="5">
         <v>9</v>
@@ -2868,13 +2871,13 @@
         <v>90</v>
       </c>
     </row>
-    <row r="42" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B42" s="33"/>
-      <c r="C42" s="36"/>
-      <c r="D42" s="43"/>
-      <c r="E42" s="43"/>
+    <row r="42" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B42" s="27"/>
+      <c r="C42" s="30"/>
+      <c r="D42" s="33"/>
+      <c r="E42" s="33"/>
       <c r="F42" s="9" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="G42" s="5">
         <v>9</v>
@@ -2890,7 +2893,7 @@
         <v>27</v>
       </c>
       <c r="K42" s="9" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="L42" s="5">
         <v>9</v>
@@ -2906,17 +2909,17 @@
         <v>27</v>
       </c>
     </row>
-    <row r="43" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B43" s="33"/>
-      <c r="C43" s="36"/>
-      <c r="D43" s="41" t="s">
-        <v>108</v>
-      </c>
-      <c r="E43" s="41" t="s">
+    <row r="43" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B43" s="27"/>
+      <c r="C43" s="30"/>
+      <c r="D43" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="E43" s="32" t="s">
         <v>66</v>
       </c>
       <c r="F43" s="9" t="s">
-        <v>132</v>
+        <v>149</v>
       </c>
       <c r="G43" s="5">
         <v>9</v>
@@ -2932,7 +2935,7 @@
         <v>360</v>
       </c>
       <c r="K43" s="9" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="L43" s="5">
         <v>9</v>
@@ -2948,13 +2951,13 @@
         <v>36</v>
       </c>
     </row>
-    <row r="44" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B44" s="33"/>
-      <c r="C44" s="36"/>
-      <c r="D44" s="43"/>
-      <c r="E44" s="43"/>
+    <row r="44" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B44" s="27"/>
+      <c r="C44" s="30"/>
+      <c r="D44" s="33"/>
+      <c r="E44" s="33"/>
       <c r="F44" s="9" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="G44" s="5">
         <v>9</v>
@@ -2970,7 +2973,7 @@
         <v>216</v>
       </c>
       <c r="K44" s="9" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="L44" s="5">
         <v>9</v>
@@ -2986,11 +2989,11 @@
         <v>72</v>
       </c>
     </row>
-    <row r="45" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B45" s="33"/>
-      <c r="C45" s="36"/>
+    <row r="45" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B45" s="27"/>
+      <c r="C45" s="30"/>
       <c r="D45" s="13" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E45" s="9" t="s">
         <v>66</v>
@@ -3012,7 +3015,7 @@
         <v>90</v>
       </c>
       <c r="K45" s="9" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="L45" s="5">
         <v>9</v>
@@ -3028,17 +3031,17 @@
         <v>27</v>
       </c>
     </row>
-    <row r="46" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B46" s="33"/>
-      <c r="C46" s="36"/>
+    <row r="46" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B46" s="27"/>
+      <c r="C46" s="30"/>
       <c r="D46" s="9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E46" s="9" t="s">
         <v>66</v>
       </c>
       <c r="F46" s="9" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G46" s="5">
         <v>9</v>
@@ -3054,7 +3057,7 @@
         <v>63</v>
       </c>
       <c r="K46" s="9" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="L46" s="5">
         <v>9</v>
@@ -3070,17 +3073,17 @@
         <v>27</v>
       </c>
     </row>
-    <row r="47" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B47" s="33"/>
-      <c r="C47" s="36"/>
+    <row r="47" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B47" s="27"/>
+      <c r="C47" s="30"/>
       <c r="D47" s="9" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E47" s="9" t="s">
         <v>66</v>
       </c>
       <c r="F47" s="9" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="G47" s="5">
         <v>9</v>
@@ -3095,9 +3098,7 @@
         <f t="shared" si="0"/>
         <v>90</v>
       </c>
-      <c r="K47" s="9" t="s">
-        <v>142</v>
-      </c>
+      <c r="K47" s="9"/>
       <c r="L47" s="5">
         <v>9</v>
       </c>
@@ -3112,17 +3113,17 @@
         <v>90</v>
       </c>
     </row>
-    <row r="48" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B48" s="34"/>
-      <c r="C48" s="37"/>
+    <row r="48" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B48" s="28"/>
+      <c r="C48" s="31"/>
       <c r="D48" s="9" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E48" s="9" t="s">
         <v>66</v>
       </c>
       <c r="F48" s="9" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="G48" s="5">
         <v>9</v>
@@ -3137,9 +3138,7 @@
         <f t="shared" si="0"/>
         <v>90</v>
       </c>
-      <c r="K48" s="9" t="s">
-        <v>142</v>
-      </c>
+      <c r="K48" s="9"/>
       <c r="L48" s="5">
         <v>9</v>
       </c>
@@ -3154,125 +3153,125 @@
         <v>90</v>
       </c>
     </row>
-    <row r="49" spans="2:15" ht="17" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B49" s="2" t="s">
         <v>44</v>
       </c>
       <c r="C49" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="D49" s="44" t="s">
+      <c r="D49" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="E49" s="45"/>
-      <c r="F49" s="45"/>
-      <c r="G49" s="45"/>
-      <c r="H49" s="45"/>
-      <c r="I49" s="45"/>
-      <c r="J49" s="45"/>
-      <c r="K49" s="45"/>
-      <c r="L49" s="45"/>
-      <c r="M49" s="45"/>
-      <c r="N49" s="45"/>
-      <c r="O49" s="46"/>
-    </row>
-    <row r="50" spans="2:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="E49" s="41"/>
+      <c r="F49" s="41"/>
+      <c r="G49" s="41"/>
+      <c r="H49" s="41"/>
+      <c r="I49" s="41"/>
+      <c r="J49" s="41"/>
+      <c r="K49" s="41"/>
+      <c r="L49" s="41"/>
+      <c r="M49" s="41"/>
+      <c r="N49" s="41"/>
+      <c r="O49" s="42"/>
+    </row>
+    <row r="50" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B50" s="5" t="s">
         <v>45</v>
       </c>
       <c r="C50" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="D50" s="47" t="s">
+      <c r="D50" s="43" t="s">
         <v>47</v>
       </c>
-      <c r="E50" s="48"/>
-      <c r="F50" s="48"/>
-      <c r="G50" s="48"/>
-      <c r="H50" s="48"/>
-      <c r="I50" s="48"/>
-      <c r="J50" s="48"/>
-      <c r="K50" s="48"/>
-      <c r="L50" s="48"/>
-      <c r="M50" s="48"/>
-      <c r="N50" s="48"/>
-      <c r="O50" s="49"/>
-    </row>
-    <row r="51" spans="2:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="E50" s="44"/>
+      <c r="F50" s="44"/>
+      <c r="G50" s="44"/>
+      <c r="H50" s="44"/>
+      <c r="I50" s="44"/>
+      <c r="J50" s="44"/>
+      <c r="K50" s="44"/>
+      <c r="L50" s="44"/>
+      <c r="M50" s="44"/>
+      <c r="N50" s="44"/>
+      <c r="O50" s="45"/>
+    </row>
+    <row r="51" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B51" s="2" t="s">
         <v>48</v>
       </c>
       <c r="C51" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="D51" s="44" t="s">
+      <c r="D51" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="E51" s="45"/>
-      <c r="F51" s="45"/>
-      <c r="G51" s="45"/>
-      <c r="H51" s="45"/>
-      <c r="I51" s="45"/>
-      <c r="J51" s="45"/>
-      <c r="K51" s="45"/>
-      <c r="L51" s="45"/>
-      <c r="M51" s="45"/>
-      <c r="N51" s="45"/>
-      <c r="O51" s="46"/>
-    </row>
-    <row r="52" spans="2:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="E51" s="41"/>
+      <c r="F51" s="41"/>
+      <c r="G51" s="41"/>
+      <c r="H51" s="41"/>
+      <c r="I51" s="41"/>
+      <c r="J51" s="41"/>
+      <c r="K51" s="41"/>
+      <c r="L51" s="41"/>
+      <c r="M51" s="41"/>
+      <c r="N51" s="41"/>
+      <c r="O51" s="42"/>
+    </row>
+    <row r="52" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B52" s="5" t="s">
         <v>50</v>
       </c>
       <c r="C52" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="D52" s="47" t="s">
+      <c r="D52" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="E52" s="48"/>
-      <c r="F52" s="48"/>
-      <c r="G52" s="48"/>
-      <c r="H52" s="48"/>
-      <c r="I52" s="48"/>
-      <c r="J52" s="48"/>
-      <c r="K52" s="48"/>
-      <c r="L52" s="48"/>
-      <c r="M52" s="48"/>
-      <c r="N52" s="48"/>
-      <c r="O52" s="49"/>
-    </row>
-    <row r="53" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B53" s="26" t="s">
+      <c r="E52" s="44"/>
+      <c r="F52" s="44"/>
+      <c r="G52" s="44"/>
+      <c r="H52" s="44"/>
+      <c r="I52" s="44"/>
+      <c r="J52" s="44"/>
+      <c r="K52" s="44"/>
+      <c r="L52" s="44"/>
+      <c r="M52" s="44"/>
+      <c r="N52" s="44"/>
+      <c r="O52" s="45"/>
+    </row>
+    <row r="53" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B53" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="C53" s="29" t="s">
+      <c r="C53" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="D53" s="38" t="s">
-        <v>110</v>
-      </c>
-      <c r="E53" s="38" t="s">
+      <c r="D53" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="E53" s="23" t="s">
         <v>66</v>
       </c>
       <c r="F53" s="7" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="G53" s="2">
         <v>9</v>
       </c>
       <c r="H53" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I53" s="2">
         <v>1</v>
       </c>
       <c r="J53" s="2">
         <f>PRODUCT(G53:I53)</f>
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="K53" s="7" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="L53" s="2">
         <v>9</v>
@@ -3288,13 +3287,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B54" s="27"/>
-      <c r="C54" s="30"/>
-      <c r="D54" s="40"/>
-      <c r="E54" s="40"/>
+    <row r="54" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B54" s="35"/>
+      <c r="C54" s="38"/>
+      <c r="D54" s="24"/>
+      <c r="E54" s="24"/>
       <c r="F54" s="7" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="G54" s="2">
         <v>9</v>
@@ -3310,7 +3309,7 @@
         <v>225</v>
       </c>
       <c r="K54" s="7" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="L54" s="2">
         <v>9</v>
@@ -3326,17 +3325,17 @@
         <v>81</v>
       </c>
     </row>
-    <row r="55" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B55" s="27"/>
-      <c r="C55" s="30"/>
-      <c r="D55" s="38" t="s">
-        <v>111</v>
-      </c>
-      <c r="E55" s="38" t="s">
+    <row r="55" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B55" s="35"/>
+      <c r="C55" s="38"/>
+      <c r="D55" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="E55" s="23" t="s">
         <v>66</v>
       </c>
       <c r="F55" s="7" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="G55" s="2">
         <v>9</v>
@@ -3352,7 +3351,7 @@
         <v>54</v>
       </c>
       <c r="K55" s="7" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="L55" s="2">
         <v>9</v>
@@ -3368,13 +3367,13 @@
         <v>36</v>
       </c>
     </row>
-    <row r="56" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B56" s="27"/>
-      <c r="C56" s="30"/>
-      <c r="D56" s="39"/>
-      <c r="E56" s="39"/>
+    <row r="56" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B56" s="35"/>
+      <c r="C56" s="38"/>
+      <c r="D56" s="25"/>
+      <c r="E56" s="25"/>
       <c r="F56" s="7" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="G56" s="2">
         <v>9</v>
@@ -3390,7 +3389,7 @@
         <v>378</v>
       </c>
       <c r="K56" s="7" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="L56" s="2">
         <v>9</v>
@@ -3406,13 +3405,13 @@
         <v>108</v>
       </c>
     </row>
-    <row r="57" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B57" s="27"/>
-      <c r="C57" s="30"/>
-      <c r="D57" s="39"/>
-      <c r="E57" s="39"/>
+    <row r="57" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B57" s="35"/>
+      <c r="C57" s="38"/>
+      <c r="D57" s="25"/>
+      <c r="E57" s="25"/>
       <c r="F57" s="7" t="s">
-        <v>115</v>
+        <v>152</v>
       </c>
       <c r="G57" s="2">
         <v>9</v>
@@ -3428,7 +3427,7 @@
         <v>126</v>
       </c>
       <c r="K57" s="7" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="L57" s="2">
         <v>9</v>
@@ -3444,13 +3443,13 @@
         <v>54</v>
       </c>
     </row>
-    <row r="58" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B58" s="28"/>
-      <c r="C58" s="31"/>
-      <c r="D58" s="40"/>
-      <c r="E58" s="40"/>
+    <row r="58" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B58" s="36"/>
+      <c r="C58" s="39"/>
+      <c r="D58" s="24"/>
+      <c r="E58" s="24"/>
       <c r="F58" s="7" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="G58" s="2">
         <v>9</v>
@@ -3466,7 +3465,7 @@
         <v>27</v>
       </c>
       <c r="K58" s="7" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="L58" s="2">
         <v>9</v>
@@ -3482,21 +3481,21 @@
         <v>27</v>
       </c>
     </row>
-    <row r="59" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B59" s="32" t="s">
+    <row r="59" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B59" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="C59" s="35" t="s">
+      <c r="C59" s="29" t="s">
         <v>57</v>
       </c>
       <c r="D59" s="13" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="E59" s="13" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="F59" s="9" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="G59" s="5">
         <v>6</v>
@@ -3526,17 +3525,17 @@
         <v>6</v>
       </c>
     </row>
-    <row r="60" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B60" s="33"/>
-      <c r="C60" s="36"/>
+    <row r="60" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B60" s="27"/>
+      <c r="C60" s="30"/>
       <c r="D60" s="13" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E60" s="13" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="F60" s="9" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G60" s="5">
         <v>6</v>
@@ -3566,17 +3565,17 @@
         <v>42</v>
       </c>
     </row>
-    <row r="61" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B61" s="34"/>
-      <c r="C61" s="37"/>
+    <row r="61" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B61" s="28"/>
+      <c r="C61" s="31"/>
       <c r="D61" s="9" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E61" s="9" t="s">
         <v>66</v>
       </c>
       <c r="F61" s="9" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="G61" s="5">
         <v>9</v>
@@ -3592,7 +3591,7 @@
         <v>630</v>
       </c>
       <c r="K61" s="9" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="L61" s="5">
         <v>9</v>
@@ -3608,21 +3607,21 @@
         <v>108</v>
       </c>
     </row>
-    <row r="62" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B62" s="26" t="s">
+    <row r="62" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B62" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="C62" s="29" t="s">
+      <c r="C62" s="37" t="s">
         <v>58</v>
       </c>
       <c r="D62" s="7" t="s">
         <v>65</v>
       </c>
       <c r="E62" s="15" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="F62" s="7" t="s">
-        <v>68</v>
+        <v>145</v>
       </c>
       <c r="G62" s="2">
         <v>6</v>
@@ -3652,17 +3651,17 @@
         <v>84</v>
       </c>
     </row>
-    <row r="63" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B63" s="27"/>
-      <c r="C63" s="30"/>
+    <row r="63" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B63" s="35"/>
+      <c r="C63" s="38"/>
       <c r="D63" s="7" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E63" s="15" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="F63" s="7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G63" s="2">
         <v>6</v>
@@ -3692,14 +3691,14 @@
         <v>42</v>
       </c>
     </row>
-    <row r="64" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B64" s="28"/>
-      <c r="C64" s="31"/>
+    <row r="64" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B64" s="36"/>
+      <c r="C64" s="39"/>
       <c r="D64" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E64" s="15" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="F64" s="7" t="s">
         <v>67</v>
@@ -3732,21 +3731,21 @@
         <v>60</v>
       </c>
     </row>
-    <row r="65" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B65" s="32" t="s">
+    <row r="65" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B65" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="C65" s="35" t="s">
+      <c r="C65" s="29" t="s">
         <v>59</v>
       </c>
       <c r="D65" s="16" t="s">
         <v>65</v>
       </c>
       <c r="E65" s="17" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="F65" s="9" t="s">
-        <v>68</v>
+        <v>145</v>
       </c>
       <c r="G65" s="5">
         <v>6</v>
@@ -3778,17 +3777,17 @@
         <v>210</v>
       </c>
     </row>
-    <row r="66" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B66" s="33"/>
-      <c r="C66" s="36"/>
+    <row r="66" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B66" s="27"/>
+      <c r="C66" s="30"/>
       <c r="D66" s="9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E66" s="17" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="F66" s="9" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G66" s="5">
         <v>6</v>
@@ -3818,14 +3817,14 @@
         <v>42</v>
       </c>
     </row>
-    <row r="67" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B67" s="34"/>
-      <c r="C67" s="37"/>
+    <row r="67" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B67" s="28"/>
+      <c r="C67" s="31"/>
       <c r="D67" s="9" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E67" s="17" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="F67" s="9" t="s">
         <v>67</v>
@@ -3858,63 +3857,63 @@
         <v>60</v>
       </c>
     </row>
-    <row r="68" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B68" s="26" t="s">
+    <row r="68" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B68" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C68" s="29" t="s">
+      <c r="C68" s="37" t="s">
         <v>62</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="E68" s="15" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F68" s="7" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="G68" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H68" s="2">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I68" s="2">
         <v>4</v>
       </c>
       <c r="J68" s="2">
         <f t="shared" si="3"/>
-        <v>200</v>
+        <v>128</v>
       </c>
       <c r="K68" s="7" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="L68" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M68" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N68" s="2">
         <v>4</v>
       </c>
       <c r="O68" s="2">
         <f t="shared" si="4"/>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="69" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B69" s="28"/>
-      <c r="C69" s="31"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="69" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B69" s="36"/>
+      <c r="C69" s="39"/>
       <c r="D69" s="7" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="E69" s="7" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="F69" s="7" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="G69" s="2">
         <v>6</v>
@@ -3944,61 +3943,61 @@
         <v>42</v>
       </c>
     </row>
-    <row r="70" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B70" s="32" t="s">
+    <row r="70" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B70" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="C70" s="35" t="s">
+      <c r="C70" s="29" t="s">
         <v>63</v>
       </c>
       <c r="D70" s="9" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="E70" s="9" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F70" s="9" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="G70" s="5">
         <v>5</v>
       </c>
       <c r="H70" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I70" s="5">
         <v>3</v>
       </c>
       <c r="J70" s="5">
         <f t="shared" si="3"/>
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="K70" s="9"/>
       <c r="L70" s="5">
         <v>5</v>
       </c>
       <c r="M70" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N70" s="5">
         <v>3</v>
       </c>
       <c r="O70" s="5">
         <f t="shared" si="4"/>
-        <v>45</v>
-      </c>
-    </row>
-    <row r="71" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B71" s="33"/>
-      <c r="C71" s="36"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="71" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B71" s="27"/>
+      <c r="C71" s="30"/>
       <c r="D71" s="18" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="E71" s="9" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F71" s="9" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="G71" s="5">
         <v>5</v>
@@ -4028,17 +4027,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B72" s="33"/>
-      <c r="C72" s="36"/>
-      <c r="D72" s="41" t="s">
-        <v>125</v>
+    <row r="72" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B72" s="27"/>
+      <c r="C72" s="30"/>
+      <c r="D72" s="32" t="s">
+        <v>119</v>
       </c>
       <c r="E72" s="9" t="s">
         <v>66</v>
       </c>
       <c r="F72" s="9" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="G72" s="5">
         <v>9</v>
@@ -4054,7 +4053,7 @@
         <v>162</v>
       </c>
       <c r="K72" s="9" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="L72" s="5">
         <v>9</v>
@@ -4070,15 +4069,15 @@
         <v>81</v>
       </c>
     </row>
-    <row r="73" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B73" s="34"/>
-      <c r="C73" s="37"/>
-      <c r="D73" s="43"/>
+    <row r="73" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B73" s="28"/>
+      <c r="C73" s="31"/>
+      <c r="D73" s="33"/>
       <c r="E73" s="9" t="s">
         <v>66</v>
       </c>
       <c r="F73" s="9" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="G73" s="5">
         <v>9</v>
@@ -4094,7 +4093,7 @@
         <v>90</v>
       </c>
       <c r="K73" s="9" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="L73" s="5">
         <v>9</v>
@@ -4110,33 +4109,33 @@
         <v>45</v>
       </c>
     </row>
-    <row r="74" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D74" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="G74" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="75" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D75" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="H75" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="76" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D76" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="I76" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="77" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:15" x14ac:dyDescent="0.25">
       <c r="E77" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="J77" t="s">
         <v>14</v>
@@ -4144,21 +4143,43 @@
     </row>
   </sheetData>
   <mergeCells count="65">
-    <mergeCell ref="E53:E54"/>
-    <mergeCell ref="D55:D58"/>
-    <mergeCell ref="B70:B73"/>
-    <mergeCell ref="C70:C73"/>
-    <mergeCell ref="D72:D73"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="B62:B64"/>
-    <mergeCell ref="C62:C64"/>
-    <mergeCell ref="B65:B67"/>
-    <mergeCell ref="C65:C67"/>
-    <mergeCell ref="B68:B69"/>
-    <mergeCell ref="C68:C69"/>
-    <mergeCell ref="E55:E58"/>
-    <mergeCell ref="B59:B61"/>
-    <mergeCell ref="C59:C61"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="L2:O2"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="B18:B22"/>
+    <mergeCell ref="C18:C22"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D29:D31"/>
+    <mergeCell ref="E29:E31"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="C7:C11"/>
+    <mergeCell ref="B7:B11"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="E9:E11"/>
+    <mergeCell ref="B33:B36"/>
+    <mergeCell ref="C33:C36"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="C38:C40"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="C29:C31"/>
     <mergeCell ref="D39:D40"/>
     <mergeCell ref="B41:B48"/>
     <mergeCell ref="C41:C48"/>
@@ -4172,43 +4193,21 @@
     <mergeCell ref="E41:E42"/>
     <mergeCell ref="D43:D44"/>
     <mergeCell ref="E43:E44"/>
-    <mergeCell ref="B33:B36"/>
-    <mergeCell ref="C33:C36"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="C38:C40"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="D29:D31"/>
-    <mergeCell ref="E29:E31"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="C7:C11"/>
-    <mergeCell ref="B7:B11"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="E9:E11"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="B18:B22"/>
-    <mergeCell ref="C18:C22"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="L2:O2"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="B62:B64"/>
+    <mergeCell ref="C62:C64"/>
+    <mergeCell ref="B65:B67"/>
+    <mergeCell ref="C65:C67"/>
+    <mergeCell ref="B59:B61"/>
+    <mergeCell ref="C59:C61"/>
+    <mergeCell ref="E53:E54"/>
+    <mergeCell ref="D55:D58"/>
+    <mergeCell ref="B70:B73"/>
+    <mergeCell ref="C70:C73"/>
+    <mergeCell ref="D72:D73"/>
+    <mergeCell ref="B68:B69"/>
+    <mergeCell ref="C68:C69"/>
+    <mergeCell ref="E55:E58"/>
   </mergeCells>
   <conditionalFormatting sqref="G53:G73 G4:G29 G30:G48">
     <cfRule type="cellIs" dxfId="5" priority="10" operator="greaterThanOrEqual">
@@ -4240,7 +4239,7 @@
       <formula>125</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="33" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="40" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>